<commit_message>
add getting sensor AVG
</commit_message>
<xml_diff>
--- a/smart_campus_site/Venue-Event (Group A).xlsx
+++ b/smart_campus_site/Venue-Event (Group A).xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3a-RPI\IC2141 Teaching materials\TM1118\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Smart Campus in W311\smart_campus_w311\smart_campus_site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C36906-76B8-48FE-BE11-411A7F2098B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B37F68-E1E8-4B13-BF58-C757CA06E563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event for Group A" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event for Group A'!$A$2:$F$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event for Group A'!$A$2:$F$51</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="23">
   <si>
     <t>ICU310</t>
   </si>
@@ -450,11 +450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,38 +1008,38 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B29" s="3">
         <v>45089</v>
       </c>
       <c r="C29" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D29" s="4">
-        <v>0.5</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B30" s="3">
         <v>45089</v>
       </c>
       <c r="C30" s="4">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D30" s="4">
         <v>0.70833333333333337</v>
@@ -1048,12 +1048,12 @@
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B31" s="3">
         <v>45089</v>
@@ -1073,16 +1073,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B32" s="3">
-        <v>45089</v>
+        <v>45090</v>
       </c>
       <c r="C32" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D32" s="4">
-        <v>0.70833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>0</v>
@@ -1093,47 +1093,47 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B33" s="3">
-        <v>45089</v>
+        <v>45090</v>
       </c>
       <c r="C33" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D33" s="4">
-        <v>0.70833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3">
         <v>45090</v>
       </c>
       <c r="C34" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="4">
-        <v>0.5</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B35" s="3">
         <v>45090</v>
@@ -1145,35 +1145,35 @@
         <v>0.5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B36" s="3">
         <v>45090</v>
       </c>
       <c r="C36" s="4">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D36" s="4">
         <v>0.70833333333333337</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" s="3">
         <v>45090</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B38" s="3">
         <v>45090</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" s="3">
         <v>45090</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="3">
         <v>45090</v>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3">
-        <v>45090</v>
+        <v>45091</v>
       </c>
       <c r="C41" s="4">
         <v>0.33333333333333331</v>
@@ -1265,44 +1265,44 @@
         <v>0.5</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B42" s="3">
-        <v>45090</v>
+        <v>45091</v>
       </c>
       <c r="C42" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D42" s="4">
-        <v>0.70833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B43" s="3">
         <v>45091</v>
       </c>
       <c r="C43" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="D43" s="4">
-        <v>0.5</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>0</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B44" s="3">
         <v>45091</v>
@@ -1328,12 +1328,12 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B45" s="3">
         <v>45091</v>
@@ -1348,12 +1348,12 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B46" s="3">
         <v>45091</v>
@@ -1365,35 +1365,35 @@
         <v>0.5</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B47" s="3">
         <v>45091</v>
       </c>
       <c r="C47" s="4">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D47" s="4">
         <v>0.70833333333333337</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B48" s="3">
         <v>45091</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B49" s="3">
         <v>45091</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B50" s="3">
         <v>45091</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B51" s="3">
         <v>45091</v>
@@ -1471,50 +1471,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="3">
-        <v>45091</v>
-      </c>
-      <c r="C52" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D52" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" s="3">
-        <v>45091</v>
-      </c>
-      <c r="C53" s="4">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D53" s="4">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:F53" xr:uid="{1FE59C04-A302-441D-A4BE-3FC73BCA2B2B}"/>
-  <sortState ref="A3:F53">
-    <sortCondition ref="B3:B53"/>
+  <autoFilter ref="A2:F51" xr:uid="{CA9A2322-A259-45DA-ACE5-F66EADAD2211}"/>
+  <sortState ref="A3:F51">
+    <sortCondition ref="B3:B51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>